<commit_message>
Erro corrigido e cadastro quase finalizado
</commit_message>
<xml_diff>
--- a/Banco de dados/SPMEDICALGROUP.xlsx
+++ b/Banco de dados/SPMEDICALGROUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10\Documents\Curso\SENAI_2S\2021-1S-2D\sprint-1-bd\exercicios\SP Medical group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40228034876\Desktop\SpMedicalGroup\Banco de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2219B13-8BB9-4DFE-AFA6-02C16D5D9D1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3A05B7-CED0-4C45-A094-248698CAD01A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="2310" windowWidth="15990" windowHeight="8535" xr2:uid="{DE495C9F-DD90-4710-8D27-4A2F27D2F19E}"/>
+    <workbookView xWindow="15420" yWindow="2310" windowWidth="15990" windowHeight="8535" firstSheet="1" activeTab="4" xr2:uid="{DE495C9F-DD90-4710-8D27-4A2F27D2F19E}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo Físico" sheetId="11" r:id="rId1"/>
@@ -627,31 +627,31 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1113,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0349CF10-AC96-4F3F-878C-185F2D565467}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1137,10 +1137,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="1"/>
       <c r="D1" s="31" t="s">
         <v>87</v>
@@ -1236,14 +1236,14 @@
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1271,10 +1271,10 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="1"/>
       <c r="D7" s="19">
         <v>1</v>
@@ -1288,7 +1288,7 @@
       <c r="G7" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="25" t="s">
         <v>96</v>
       </c>
       <c r="I7" s="9">
@@ -1316,7 +1316,7 @@
       <c r="G8" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I8" s="9">
@@ -1344,7 +1344,7 @@
       <c r="G9" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="25" t="s">
         <v>98</v>
       </c>
       <c r="I9" s="9">
@@ -1372,7 +1372,7 @@
       <c r="G10" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="25" t="s">
         <v>99</v>
       </c>
       <c r="I10" s="9">
@@ -1400,7 +1400,7 @@
       <c r="G11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="25" t="s">
         <v>100</v>
       </c>
       <c r="I11" s="9">
@@ -1428,7 +1428,7 @@
       <c r="G12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="25" t="s">
         <v>101</v>
       </c>
       <c r="I12" s="9">
@@ -1456,7 +1456,7 @@
       <c r="G13" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="25" t="s">
         <v>98</v>
       </c>
       <c r="I13" s="9">
@@ -1484,7 +1484,7 @@
       <c r="G14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="25" t="s">
         <v>102</v>
       </c>
       <c r="I14" s="9">
@@ -1512,7 +1512,7 @@
       <c r="G15" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="25" t="s">
         <v>103</v>
       </c>
       <c r="I15" s="9">
@@ -1540,7 +1540,7 @@
       <c r="G16" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="25" t="s">
         <v>104</v>
       </c>
       <c r="I16" s="9">
@@ -1568,7 +1568,7 @@
       <c r="G17" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="25" t="s">
         <v>105</v>
       </c>
       <c r="I17" s="9">
@@ -1600,13 +1600,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
@@ -1738,13 +1738,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
@@ -1771,10 +1771,10 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10">
         <v>1</v>
@@ -1958,14 +1958,14 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,7 +2191,7 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,7 +2402,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,8 +2567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AF3780-D385-44F7-991E-BFAF92DA9865}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672D278F-6B70-445D-80C8-43CA14EAD461}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2951,7 +2951,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>